<commit_message>
final PCB ovladaci karta
</commit_message>
<xml_diff>
--- a/PCB_ovladaci_karta/Ovladaci_karta/Project Outputs for Ovladaci_karta/BOM/Copy of Bill of Materials-Ovladaci_karta.xlsx
+++ b/PCB_ovladaci_karta/Ovladaci_karta/Project Outputs for Ovladaci_karta/BOM/Copy of Bill of Materials-Ovladaci_karta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip\Desktop\diplomka\PCB_ovladaci_karta\Ovladaci_karta\Project Outputs for Ovladaci_karta\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{863C1295-3D4B-48BF-AF05-CE5260A681E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B06163EA-5CD2-47A7-9E44-79F4B993C5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="4980" windowWidth="45270" windowHeight="26310" xr2:uid="{40C6E08A-A636-47C4-A554-CA2C57C8EF86}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="45270" windowHeight="26310" xr2:uid="{E0ABDCD2-0D16-4FC2-94A2-37200ECE597F}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of Bill of Materials-Ovlad" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="293">
   <si>
     <t>Designator</t>
   </si>
@@ -510,16 +510,16 @@
     <t>R43</t>
   </si>
   <si>
-    <t>ERJ-S02F2203X</t>
-  </si>
-  <si>
-    <t>220k</t>
-  </si>
-  <si>
-    <t>Resistor - 0402 -  220k - 1% - 100mW</t>
-  </si>
-  <si>
-    <t>https://cz.mouser.com/ProductDetail/TE-Connectivity-Holsworthy/CRGCQ0402F220K?qs=wUXugUrL1qxgaPkTarsp4Q%3D%3D</t>
+    <t>ERJ2RKD2323X</t>
+  </si>
+  <si>
+    <t>232k</t>
+  </si>
+  <si>
+    <t>Resistor - 0402 -  232k - 0.5% - 62mW</t>
+  </si>
+  <si>
+    <t>https://cz.mouser.com/ProductDetail/Panasonic/ERJ2RKD2323X?qs=YCa%2FAAYMW02KvIWpqTK%252Bgg%3D%3D</t>
   </si>
   <si>
     <t>R5, R15_U_PORT_SINGLE1, R15_U_PORT_SINGLE2, R15_U_PORT_SINGLE3, R16_U_PORT_SINGLE1, R16_U_PORT_SINGLE2, R16_U_PORT_SINGLE3, R17_U_PORT_SINGLE1, R17_U_PORT_SINGLE2, R17_U_PORT_SINGLE3, R23, R24_U_PORT_SINGLE1, R24_U_PORT_SINGLE2, R24_U_PORT_SINGLE3, R26_U_PORT_SINGLE1, R26_U_PORT_SINGLE2, R26_U_PORT_SINGLE3, R37_U_PORT_SINGLE1, R37_U_PORT_SINGLE2, R37_U_PORT_SINGLE3, R39_U_PORT_SINGLE1, R39_U_PORT_SINGLE2, R39_U_PORT_SINGLE3, R40_U_PORT_SINGLE1, R40_U_PORT_SINGLE2, R40_U_PORT_SINGLE3</t>
@@ -1283,7 +1283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C0EE83-760B-4BF4-B7E9-2ADA19BA2E0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8037A38-9308-4FC7-BB8E-8F85E2D1ED56}">
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -2451,10 +2451,18 @@
       <c r="H27" s="1">
         <v>1</v>
       </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
+      <c r="I27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.12243</v>
+      </c>
+      <c r="K27" s="1">
+        <v>21020</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0.12243</v>
+      </c>
       <c r="M27" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>